<commit_message>
Final report: Added resutls + discussion
</commit_message>
<xml_diff>
--- a/Final Report/results/results_random_density2.xlsx
+++ b/Final Report/results/results_random_density2.xlsx
@@ -714,58 +714,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,58 +884,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1054,58 +1054,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1224,58 +1224,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1353,15 +1353,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190519872"/>
-        <c:axId val="190520432"/>
+        <c:axId val="185207968"/>
+        <c:axId val="185208528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190519872"/>
+        <c:axId val="185207968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="9.5"/>
-          <c:min val="0"/>
+          <c:max val="28"/>
+          <c:min val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1479,12 +1479,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190520432"/>
+        <c:crossAx val="185208528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190520432"/>
+        <c:axId val="185208528"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1603,7 +1603,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190519872"/>
+        <c:crossAx val="185207968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1824,58 +1824,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1994,58 +1994,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2164,58 +2164,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2334,58 +2334,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2463,11 +2463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190345040"/>
-        <c:axId val="190345600"/>
+        <c:axId val="185211328"/>
+        <c:axId val="185211888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190345040"/>
+        <c:axId val="185211328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.5"/>
@@ -2589,12 +2589,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190345600"/>
+        <c:crossAx val="185211888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190345600"/>
+        <c:axId val="185211888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600000000000"/>
@@ -2713,7 +2713,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190345040"/>
+        <c:crossAx val="185211328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4240,8 +4240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4260,8 +4260,8 @@
         <v>178721554</v>
       </c>
       <c r="D1">
-        <f>(B1+1)*0.5</f>
-        <v>0.5</v>
+        <f t="shared" ref="D1:D17" si="0">B1+10</f>
+        <v>10</v>
       </c>
       <c r="E1">
         <v>0.3</v>
@@ -4276,8 +4276,8 @@
         <v>85218832</v>
       </c>
       <c r="J1">
-        <f>(H1+1)*0.5</f>
-        <v>0.5</v>
+        <f t="shared" ref="J1:J17" si="1">H1+10</f>
+        <v>10</v>
       </c>
       <c r="K1">
         <v>0.3</v>
@@ -4292,8 +4292,8 @@
         <v>128442854</v>
       </c>
       <c r="P1">
-        <f>(N1+1)*0.5</f>
-        <v>0.5</v>
+        <f t="shared" ref="P1:P17" si="2">N1+10</f>
+        <v>10</v>
       </c>
       <c r="Q1">
         <v>0.3</v>
@@ -4308,8 +4308,8 @@
         <v>117506743</v>
       </c>
       <c r="V1">
-        <f>(T1+1)*0.5</f>
-        <v>0.5</v>
+        <f t="shared" ref="V1:V17" si="3">T1+10</f>
+        <v>10</v>
       </c>
       <c r="W1">
         <v>0.3</v>
@@ -4326,8 +4326,8 @@
         <v>195980010</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D18" si="0">(B2+1)*0.5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>0.3</v>
@@ -4342,8 +4342,8 @@
         <v>386043388</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J18" si="1">(H2+1)*0.5</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="K2">
         <v>0.3</v>
@@ -4358,8 +4358,8 @@
         <v>452009315</v>
       </c>
       <c r="P2">
-        <f t="shared" ref="P2:P18" si="2">(N2+1)*0.5</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="Q2">
         <v>0.3</v>
@@ -4374,8 +4374,8 @@
         <v>114305120</v>
       </c>
       <c r="V2">
-        <f t="shared" ref="V2:V18" si="3">(T2+1)*0.5</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>11</v>
       </c>
       <c r="W2">
         <v>0.3</v>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>0.3</v>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="J3">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>12</v>
       </c>
       <c r="K3">
         <v>0.3</v>
@@ -4425,7 +4425,7 @@
       </c>
       <c r="P3">
         <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>12</v>
       </c>
       <c r="Q3">
         <v>0.3</v>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="V3">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>12</v>
       </c>
       <c r="W3">
         <v>0.3</v>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>0.3</v>
@@ -4475,7 +4475,7 @@
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="K4">
         <v>0.3</v>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="Q4">
         <v>0.3</v>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="V4">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="W4">
         <v>0.3</v>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>0.3</v>
@@ -4541,7 +4541,7 @@
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="K5">
         <v>0.3</v>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="Q5">
         <v>0.3</v>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="V5">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>14</v>
       </c>
       <c r="W5">
         <v>0.3</v>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>0.3</v>
@@ -4607,7 +4607,7 @@
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="K6">
         <v>0.3</v>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="P6">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="Q6">
         <v>0.3</v>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="V6">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="W6">
         <v>0.3</v>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>0.3</v>
@@ -4673,7 +4673,7 @@
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>16</v>
       </c>
       <c r="K7">
         <v>0.3</v>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="P7">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>16</v>
       </c>
       <c r="Q7">
         <v>0.3</v>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="V7">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>16</v>
       </c>
       <c r="W7">
         <v>0.3</v>
@@ -4723,7 +4723,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>0.3</v>
@@ -4739,7 +4739,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="K8">
         <v>0.3</v>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="P8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Q8">
         <v>0.3</v>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="V8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="W8">
         <v>0.3</v>
@@ -4789,7 +4789,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>0.3</v>
@@ -4805,7 +4805,7 @@
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>18</v>
       </c>
       <c r="K9">
         <v>0.3</v>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="P9">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>18</v>
       </c>
       <c r="Q9">
         <v>0.3</v>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="V9">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>18</v>
       </c>
       <c r="W9">
         <v>0.3</v>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>0.3</v>
@@ -4871,7 +4871,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="K10">
         <v>0.3</v>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="Q10">
         <v>0.3</v>
@@ -4903,7 +4903,7 @@
       </c>
       <c r="V10">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="W10">
         <v>0.3</v>
@@ -4921,7 +4921,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>0.3</v>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>20</v>
       </c>
       <c r="K11">
         <v>0.3</v>
@@ -4953,7 +4953,7 @@
       </c>
       <c r="P11">
         <f t="shared" si="2"/>
-        <v>5.5</v>
+        <v>20</v>
       </c>
       <c r="Q11">
         <v>0.3</v>
@@ -4969,7 +4969,7 @@
       </c>
       <c r="V11">
         <f t="shared" si="3"/>
-        <v>5.5</v>
+        <v>20</v>
       </c>
       <c r="W11">
         <v>0.3</v>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>0.3</v>
@@ -5003,7 +5003,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="K12">
         <v>0.3</v>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="P12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="Q12">
         <v>0.3</v>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="V12">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="W12">
         <v>0.3</v>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <v>0.3</v>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>22</v>
       </c>
       <c r="K13">
         <v>0.3</v>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="P13">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>22</v>
       </c>
       <c r="Q13">
         <v>0.3</v>
@@ -5101,7 +5101,7 @@
       </c>
       <c r="V13">
         <f t="shared" si="3"/>
-        <v>6.5</v>
+        <v>22</v>
       </c>
       <c r="W13">
         <v>0.3</v>
@@ -5119,7 +5119,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E14">
         <v>0.3</v>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="K14">
         <v>0.3</v>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="Q14">
         <v>0.3</v>
@@ -5167,7 +5167,7 @@
       </c>
       <c r="V14">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="W14">
         <v>0.3</v>
@@ -5185,7 +5185,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="E15">
         <v>0.3</v>
@@ -5201,7 +5201,7 @@
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="K15">
         <v>0.3</v>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="P15">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="Q15">
         <v>0.3</v>
@@ -5233,7 +5233,7 @@
       </c>
       <c r="V15">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="W15">
         <v>0.3</v>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>0.3</v>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K16">
         <v>0.3</v>
@@ -5283,7 +5283,7 @@
       </c>
       <c r="P16">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="Q16">
         <v>0.3</v>
@@ -5299,7 +5299,7 @@
       </c>
       <c r="V16">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="W16">
         <v>0.3</v>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>8.5</v>
+        <v>26</v>
       </c>
       <c r="E17">
         <v>0.3</v>
@@ -5333,7 +5333,7 @@
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>26</v>
       </c>
       <c r="K17">
         <v>0.3</v>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="P17">
         <f t="shared" si="2"/>
-        <v>8.5</v>
+        <v>26</v>
       </c>
       <c r="Q17">
         <v>0.3</v>
@@ -5365,7 +5365,7 @@
       </c>
       <c r="V17">
         <f t="shared" si="3"/>
-        <v>8.5</v>
+        <v>26</v>
       </c>
       <c r="W17">
         <v>0.3</v>
@@ -5382,8 +5382,8 @@
         <v>12950121276</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>B18+10</f>
+        <v>27</v>
       </c>
       <c r="E18">
         <v>0.3</v>
@@ -5398,8 +5398,8 @@
         <v>223449291287</v>
       </c>
       <c r="J18">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>H18+10</f>
+        <v>27</v>
       </c>
       <c r="K18">
         <v>0.3</v>
@@ -5414,8 +5414,8 @@
         <v>219788435398</v>
       </c>
       <c r="P18">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f>N18+10</f>
+        <v>27</v>
       </c>
       <c r="Q18">
         <v>0.3</v>
@@ -5430,8 +5430,8 @@
         <v>496629871751</v>
       </c>
       <c r="V18">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f>T18+10</f>
+        <v>27</v>
       </c>
       <c r="W18">
         <v>0.3</v>

</xml_diff>